<commit_message>
quantitative evaluation plots and execution metrics analtsis
</commit_message>
<xml_diff>
--- a/test-code-generator/Evaluation/Results/quantitative_analysis_results.xlsx
+++ b/test-code-generator/Evaluation/Results/quantitative_analysis_results.xlsx
@@ -2876,51 +2876,55 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C12" t="n">
-        <v>44.44444444444444</v>
+        <v>88.88888888888889</v>
       </c>
       <c r="D12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E12" t="n">
-        <v>55.55555555555556</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="F12" t="n">
-        <v>44.44444444444444</v>
+        <v>88.88888888888889</v>
       </c>
       <c r="G12" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="H12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
         <v>18</v>
       </c>
       <c r="J12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="K12" t="n">
-        <v>44.44444444444444</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="L12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="M12" t="n">
-        <v>55.55555555555556</v>
-      </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
+        <v>11.11111111111111</v>
+      </c>
+      <c r="N12" t="n">
+        <v>9</v>
+      </c>
+      <c r="O12" t="n">
+        <v>50</v>
+      </c>
       <c r="P12" t="n">
-        <v>44.44444444444444</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="Q12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="R12" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S12" t="n">
         <v>18</v>
@@ -2932,25 +2936,25 @@
         <v>55.55555555555556</v>
       </c>
       <c r="V12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W12" t="n">
-        <v>5.555555555555555</v>
+        <v>16.66666666666666</v>
       </c>
       <c r="X12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Y12" t="n">
-        <v>38.88888888888889</v>
+        <v>27.77777777777778</v>
       </c>
       <c r="Z12" t="n">
-        <v>38.88888888888889</v>
+        <v>27.77777777777778</v>
       </c>
       <c r="AA12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AB12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AC12" t="n">
         <v>18</v>
@@ -3247,13 +3251,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>44.44444444444444</v>
+        <v>88.88888888888889</v>
       </c>
       <c r="C12" t="n">
-        <v>44.44444444444444</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="D12" t="n">
-        <v>38.88888888888889</v>
+        <v>27.77777777777778</v>
       </c>
     </row>
     <row r="13">
@@ -6431,7 +6435,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -6483,12 +6487,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -6545,12 +6549,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -6581,12 +6585,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E9" t="n">
@@ -6607,17 +6611,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -6638,12 +6642,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -6669,12 +6673,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -6700,12 +6704,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -6731,12 +6735,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -6762,12 +6766,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -6793,12 +6797,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -6886,17 +6890,17 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E19" t="n">
@@ -8296,51 +8300,55 @@
         <v>0.9380770128604092</v>
       </c>
       <c r="N12" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O12" t="n">
-        <v>44.44444444444444</v>
+        <v>88.88888888888889</v>
       </c>
       <c r="P12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="Q12" t="n">
-        <v>55.55555555555556</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="R12" t="n">
-        <v>44.44444444444444</v>
+        <v>88.88888888888889</v>
       </c>
       <c r="S12" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="T12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="U12" t="n">
         <v>18</v>
       </c>
       <c r="V12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W12" t="n">
-        <v>44.44444444444444</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="X12" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="Y12" t="n">
-        <v>55.55555555555556</v>
-      </c>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
+        <v>11.11111111111111</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>50</v>
+      </c>
       <c r="AB12" t="n">
-        <v>44.44444444444444</v>
+        <v>38.88888888888889</v>
       </c>
       <c r="AC12" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AD12" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AE12" t="n">
         <v>18</v>
@@ -8352,25 +8360,25 @@
         <v>55.55555555555556</v>
       </c>
       <c r="AH12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AI12" t="n">
-        <v>5.555555555555555</v>
+        <v>16.66666666666666</v>
       </c>
       <c r="AJ12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AK12" t="n">
-        <v>38.88888888888889</v>
+        <v>27.77777777777778</v>
       </c>
       <c r="AL12" t="n">
-        <v>38.88888888888889</v>
+        <v>27.77777777777778</v>
       </c>
       <c r="AM12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AN12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AO12" t="n">
         <v>18</v>

</xml_diff>